<commit_message>
Tax,Discount and Price list added to sales module
</commit_message>
<xml_diff>
--- a/MavenBook/src/test/resources/CustomerData.xlsx
+++ b/MavenBook/src/test/resources/CustomerData.xlsx
@@ -129,18 +129,9 @@
     <t>Mr</t>
   </si>
   <si>
-    <t>Subin</t>
-  </si>
-  <si>
     <t>Mathew</t>
   </si>
   <si>
-    <t>subin.polosys@yahoo.com</t>
-  </si>
-  <si>
-    <t>subin.polosys2@yahoo.com</t>
-  </si>
-  <si>
     <t>VAT Registered</t>
   </si>
   <si>
@@ -198,9 +189,6 @@
     <t>Company Disp Name(Arabic)</t>
   </si>
   <si>
-    <t>355458489378523</t>
-  </si>
-  <si>
     <t>9942000355</t>
   </si>
   <si>
@@ -213,20 +201,32 @@
     <t>Mr.</t>
   </si>
   <si>
-    <t>Automated</t>
-  </si>
-  <si>
-    <t>Automated Test</t>
-  </si>
-  <si>
-    <t>Automated one</t>
+    <t>Sujith</t>
+  </si>
+  <si>
+    <t>sujith.polosys@yahoo.com</t>
+  </si>
+  <si>
+    <t>sujith.polosys2@yahoo.com</t>
+  </si>
+  <si>
+    <t>355458489378423</t>
+  </si>
+  <si>
+    <t>Contact FName</t>
+  </si>
+  <si>
+    <t>Contact LName</t>
+  </si>
+  <si>
+    <t>Contact Salutation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,6 +280,14 @@
       <name val="Lucida Fax"/>
       <family val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -298,10 +306,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -319,8 +328,10 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -626,10 +637,10 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:X29"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="T26" sqref="T26"/>
+      <selection pane="bottomLeft" activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -678,7 +689,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>5</v>
@@ -735,72 +746,72 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>40</v>
+        <v>61</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>63</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="K2" s="14">
         <v>100</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="Q2" s="14">
         <v>100</v>
       </c>
       <c r="R2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="V2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:24" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -955,11 +966,12 @@
       <c r="J29" s="15"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="H2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="M2" numberStoredAsText="1"/>
-  </ignoredErrors>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -969,7 +981,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1028,25 +1040,25 @@
         <v>36</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="I2" s="14">
         <v>452102</v>
@@ -1164,12 +1176,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomLeft" activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="21.140625" style="10" customWidth="1"/>
@@ -1180,19 +1192,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>1</v>
+        <v>65</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>34</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>35</v>
@@ -1200,16 +1212,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E2" s="15">
         <v>4561320789</v>

</xml_diff>